<commit_message>
unity 3d for prototype
</commit_message>
<xml_diff>
--- a/schedule2013-10-14.xlsx
+++ b/schedule2013-10-14.xlsx
@@ -524,7 +524,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -541,17 +541,17 @@
         <v>1</v>
       </c>
       <c r="B1" s="4">
-        <v>0.22916666666666666</v>
+        <v>0.24305555555555555</v>
       </c>
       <c r="C1" s="5">
-        <v>0.24305555555555555</v>
+        <v>0.25</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="4">
         <f>C1-B1</f>
-        <v>1.3888888888888895E-2</v>
+        <v>6.9444444444444475E-3</v>
       </c>
       <c r="F1" s="3">
         <v>1</v>
@@ -563,7 +563,7 @@
       </c>
       <c r="B2" s="10">
         <f>C1</f>
-        <v>0.24305555555555555</v>
+        <v>0.25</v>
       </c>
       <c r="C2" s="11">
         <v>0.3125</v>
@@ -573,7 +573,7 @@
       </c>
       <c r="E2" s="10">
         <f t="shared" ref="E2:E15" si="0">C2-B2</f>
-        <v>6.9444444444444448E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F2" s="9">
         <v>2</v>
@@ -808,14 +808,14 @@
         <v>0.79861111111111116</v>
       </c>
       <c r="C13" s="5">
-        <v>0.84027777777777779</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
+        <v>5.5555555555555469E-2</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -827,10 +827,10 @@
       </c>
       <c r="B14" s="10">
         <f t="shared" si="1"/>
-        <v>0.84027777777777779</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="C14" s="11">
-        <v>0.91666666666666663</v>
+        <v>0.93055555555555547</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>0</v>
@@ -849,10 +849,10 @@
       </c>
       <c r="B15" s="10">
         <f t="shared" si="1"/>
-        <v>0.91666666666666663</v>
+        <v>0.93055555555555547</v>
       </c>
       <c r="C15" s="11">
-        <v>0.9375</v>
+        <v>0.95138888888888884</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>10</v>
@@ -871,11 +871,11 @@
       </c>
       <c r="B16" s="7">
         <f>C15</f>
-        <v>0.9375</v>
+        <v>0.95138888888888884</v>
       </c>
       <c r="C16" s="8">
         <f>B1</f>
-        <v>0.22916666666666666</v>
+        <v>0.24305555555555555</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>4</v>
@@ -898,7 +898,7 @@
       <c r="C18" s="17"/>
       <c r="E18" s="18">
         <f>SUMIF(F$1:F$16,F18,E$1:E$16)</f>
-        <v>0.1875</v>
+        <v>0.19444444444444439</v>
       </c>
       <c r="F18" s="19">
         <v>1</v>
@@ -909,7 +909,7 @@
       <c r="C19" s="14"/>
       <c r="E19" s="20">
         <f t="shared" ref="E19:E20" si="2">SUMIF(F$1:F$16,F19,E$1:E$16)</f>
-        <v>0.47916666666666663</v>
+        <v>0.47222222222222215</v>
       </c>
       <c r="F19" s="21">
         <v>2</v>

</xml_diff>